<commit_message>
Fix bug export file when deploy
</commit_message>
<xml_diff>
--- a/WebSiteBanHang/FilesUpload/DanhSachDonHang.xlsx
+++ b/WebSiteBanHang/FilesUpload/DanhSachDonHang.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Mã đơn hàng</t>
   </si>
@@ -32,124 +32,94 @@
     <t>Trạng thái</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>1000000</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn A</t>
-  </si>
-  <si>
-    <t>10/5/2019</t>
-  </si>
-  <si>
-    <t>05/8/2019</t>
+    <t>19</t>
+  </si>
+  <si>
+    <t>587000</t>
+  </si>
+  <si>
+    <t>Lê Kim Phi</t>
+  </si>
+  <si>
+    <t>15/12/2020</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>3000000</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn Anh</t>
-  </si>
-  <si>
-    <t>11/5/2019</t>
-  </si>
-  <si>
-    <t>05/7/2019</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>200000</t>
-  </si>
-  <si>
-    <t>15/5/2019</t>
-  </si>
-  <si>
-    <t>07/10/2019</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>2500000</t>
-  </si>
-  <si>
-    <t>Lê Kim Phi</t>
-  </si>
-  <si>
-    <t>04/5/2019</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>2000000</t>
-  </si>
-  <si>
-    <t>03/5/2019</t>
-  </si>
-  <si>
-    <t>21/5/2019</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>258000</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>247000</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>608000</t>
-  </si>
-  <si>
-    <t>23/5/2019</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>139000</t>
-  </si>
-  <si>
-    <t>22/5/2019</t>
-  </si>
-  <si>
-    <t>18</t>
+    <t>20</t>
+  </si>
+  <si>
+    <t>534000</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>468791</t>
+  </si>
+  <si>
+    <t>16/12/2020</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>529000</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>387000</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>356000</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>566500</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>259000</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>369791</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>517000</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
   <si>
     <t>69500</t>
   </si>
   <si>
-    <t>17/5/2019</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>100000</t>
-  </si>
-  <si>
-    <t>09/5/2019</t>
+    <t>Mai xinh gai 202</t>
+  </si>
+  <si>
+    <t>24/12/2020</t>
+  </si>
+  <si>
+    <t>31</t>
   </si>
 </sst>
 </file>
@@ -213,7 +183,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" state="frozen" activePane="bottomLeft"/>
@@ -267,236 +237,248 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1"/>
@@ -634,6 +616,14 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
+    <row r="32" ht="30" customHeight="1">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>